<commit_message>
Revert "Revert "Merge branch 'main' into yoshikawa""
This reverts commit 7cce9d767ac59098fa8b65984c3372c18bce31f5.
</commit_message>
<xml_diff>
--- a/試験設計書/試験項目書_試験結果一覧画面.xlsx
+++ b/試験設計書/試験項目書_試験結果一覧画面.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{B32B892F-6AEA-45A0-A930-7B1A1A8E1609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F49F391E-052D-4380-9CA1-95D521B3336F}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{B32B892F-6AEA-45A0-A930-7B1A1A8E1609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA68B206-92B0-4C2F-9FBD-DA35D5A69B3B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="単体試験項目書" sheetId="11" r:id="rId1"/>
     <sheet name="結合試験項目書" sheetId="10" r:id="rId2"/>
+    <sheet name="試験写真" sheetId="12" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1"/>
@@ -301,6 +302,9 @@
   <si>
     <t>過去の試験結果　　　　　　　②ない</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -695,6 +699,1039 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7771311" cy="3666768"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6232108E-591D-476D-8C0E-B0C26B58045E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="304800"/>
+          <a:ext cx="7771311" cy="3666768"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7771311" cy="3582590"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B94E883-207F-4605-80AB-5BBA7796E2EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4785360"/>
+          <a:ext cx="7771311" cy="3582590"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="直線コネクタ 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E41BA45-7930-4302-B1D4-4360AE87854D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3421380" y="2118360"/>
+          <a:ext cx="601980" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1059180</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="直線コネクタ 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67296E3A-6E59-48BF-8B5D-79598F24D963}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2011680" y="3512820"/>
+          <a:ext cx="594360" cy="15240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1325880</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直線コネクタ 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0A3B043-CF1B-4E89-AB57-8D03B3EAF756}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3322320" y="6667500"/>
+          <a:ext cx="701040" cy="15240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>830580</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>845820</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直線コネクタ 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D12237D5-F235-4FD4-8681-294EA909D45E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2011680" y="7315200"/>
+          <a:ext cx="670560" cy="15240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7771311" cy="3647360"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="図 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3701B64-97DC-4FCB-BD8B-4ACD2A9744CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9159240"/>
+          <a:ext cx="7771311" cy="3647360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7771311" cy="3635216"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="図 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72F3B0F0-BB2C-488E-9C6C-EC22543545ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="13266420"/>
+          <a:ext cx="7771311" cy="3635216"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1348740</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="楕円 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62502AEC-1EDD-4437-A185-9193A99A30CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3413760" y="9532620"/>
+          <a:ext cx="609600" cy="701040"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="テキスト ボックス 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1444CEDD-A1BE-4205-ABF1-C699BBDE9305}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4023360" y="9669780"/>
+          <a:ext cx="1623060" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600"/>
+            <a:t>ここをクリックと</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>297690</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>26934</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>208074</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>67244</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="矢印: 左カーブ 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFA0F900-118B-4A08-96F3-1FB4A2962B93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1583326">
+          <a:off x="4321050" y="10085334"/>
+          <a:ext cx="1251504" cy="4383710"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedLeftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1" cap="none" spc="50">
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst>
+              <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                <a:srgbClr val="000000">
+                  <a:alpha val="50000"/>
+                </a:srgbClr>
+              </a:innerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7771311" cy="3647360"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="図 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C824B95-0CDB-4AC6-A919-6B12A5C4B4D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="18051780"/>
+          <a:ext cx="7771311" cy="3647360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1455420</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="テキスト ボックス 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD760CE4-FFAF-4587-82FF-11D5099D61DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4023360" y="20939760"/>
+          <a:ext cx="1859280" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600"/>
+            <a:t>ここをクリックと</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1341120</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="楕円 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{968BEA94-6BDB-40A2-B6C9-A5481BDAD0F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3406140" y="20718780"/>
+          <a:ext cx="617220" cy="701040"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7771311" cy="3610927"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="図 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FE4B6DF-6189-4619-A112-2ED5F684DF9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="22456140"/>
+          <a:ext cx="7771311" cy="3610927"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1797578</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>23280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276867</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>129960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="矢印: 下 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08D6D683-D70B-4253-9613-3E6077554B86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1207983">
+          <a:off x="4022618" y="21283080"/>
+          <a:ext cx="277609" cy="1935480"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>670560</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1463040</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>205740</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="楕円 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A0232BD-F344-43A5-878D-AB60A8E98FA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4023360" y="19583400"/>
+          <a:ext cx="0" cy="510540"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1440180</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="楕円 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10459FBC-6763-4D55-9F87-5D829124928B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4000500" y="23347680"/>
+          <a:ext cx="22860" cy="510540"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -986,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C08A44E2-5283-45D2-8C70-BFE4D440D314}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1063,7 +2100,9 @@
       <c r="D4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F4" s="14" t="s">
         <v>25</v>
       </c>
@@ -1081,7 +2120,9 @@
       <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F5" s="14" t="s">
         <v>28</v>
       </c>
@@ -1106,11 +2147,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.2"/>
@@ -1187,7 +2228,9 @@
       <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1203,7 +2246,9 @@
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1219,7 +2264,9 @@
       <c r="D6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F6" s="14" t="s">
         <v>26</v>
       </c>
@@ -1237,7 +2284,9 @@
       <c r="D7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F7" s="14" t="s">
         <v>27</v>
       </c>
@@ -1305,11 +2354,104 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E8 E10:E13" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E13 E4:E8" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"OK,NG,実施不可"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC82F3D6-5F72-49F7-AE8C-2B58D978A379}">
+  <dimension ref="A1:F77"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J104" sqref="J104"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="64.8" x14ac:dyDescent="0.2">
+      <c r="A1" s="13">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="48.6" x14ac:dyDescent="0.2">
+      <c r="A20" s="13">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="32.4" x14ac:dyDescent="0.2">
+      <c r="A39" s="13">
+        <v>3</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="32.4" x14ac:dyDescent="0.2">
+      <c r="A77" s="13">
+        <v>4</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E20" xr:uid="{2A42E21F-FCD4-470D-B7C5-1011473F3AC0}">
+      <formula1>"OK,NG,実施不可"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>